<commit_message>
Sorting of Files, addition of a moving ROI for the Fall
Changes were made to the region of interest for the fall. It is now possible to automatically change the ROI by shifting it by the displacemnt from the previous image pair. This part is still under development but should work fine.

Also the files were sorted for Federica and for developing.
</commit_message>
<xml_diff>
--- a/PIV_Campaign_Processing/Observation_periods.xlsx
+++ b/PIV_Campaign_Processing/Observation_periods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manue\Documents\GitHub\ratzVKI\PIV_Campaign_Processing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ratzVKI\PIV_Campaign_Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCB2A72C-DC02-4D67-B7D1-BD23BFE3879A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CA47A5-307D-4B29-836A-0150CCD099DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9530F36F-8309-4E2A-8AEF-06175DE3F285}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9530F36F-8309-4E2A-8AEF-06175DE3F285}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>F_h1_f1000_1_q</t>
   </si>
@@ -149,13 +149,16 @@
     <t>Start of fall</t>
   </si>
   <si>
-    <t>Interface appearing</t>
-  </si>
-  <si>
     <t>Last good image (probably)</t>
   </si>
   <si>
     <t>Refering to index image</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>Last image with full ROI</t>
   </si>
 </sst>
 </file>
@@ -513,29 +516,29 @@
   <dimension ref="B1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -543,16 +546,16 @@
         <v>1300</v>
       </c>
       <c r="D2" s="1">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="E2" s="1">
         <v>1651</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -560,13 +563,13 @@
         <v>315</v>
       </c>
       <c r="D3" s="1">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="E3" s="1">
         <v>930</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -574,13 +577,13 @@
         <v>560</v>
       </c>
       <c r="D4" s="1">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E4" s="1">
         <v>801</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -588,13 +591,13 @@
         <v>620</v>
       </c>
       <c r="D5" s="1">
-        <v>899</v>
+        <v>893</v>
       </c>
       <c r="E5" s="1">
         <v>1061</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -602,18 +605,24 @@
         <v>153</v>
       </c>
       <c r="D6" s="1">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E6" s="1">
         <v>379</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -621,13 +630,13 @@
         <v>220</v>
       </c>
       <c r="D8" s="1">
-        <v>397</v>
+        <v>377</v>
       </c>
       <c r="E8" s="1">
         <v>462</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -641,7 +650,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -649,13 +658,13 @@
         <v>445</v>
       </c>
       <c r="D10" s="1">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E10" s="1">
         <v>642</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -663,18 +672,18 @@
         <v>520</v>
       </c>
       <c r="D11" s="1">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="E11" s="1">
         <v>1073</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -682,7 +691,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -690,7 +699,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -698,7 +707,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -706,7 +715,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -714,7 +723,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>15</v>
       </c>
@@ -722,7 +731,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>16</v>
       </c>
@@ -730,7 +739,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>17</v>
       </c>
@@ -738,7 +747,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -746,7 +755,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>19</v>
       </c>
@@ -754,7 +763,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>20</v>
       </c>
@@ -762,7 +771,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>21</v>
       </c>
@@ -770,7 +779,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>22</v>
       </c>
@@ -778,7 +787,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>23</v>
       </c>
@@ -786,7 +795,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>24</v>
       </c>
@@ -794,7 +803,7 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>25</v>
       </c>
@@ -802,7 +811,7 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>26</v>
       </c>
@@ -810,7 +819,7 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>27</v>
       </c>
@@ -818,7 +827,7 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>28</v>
       </c>
@@ -826,7 +835,7 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>29</v>
       </c>
@@ -834,7 +843,7 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>30</v>
       </c>
@@ -842,7 +851,7 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>31</v>
       </c>
@@ -850,7 +859,7 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>32</v>
       </c>
@@ -858,7 +867,7 @@
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>33</v>
       </c>
@@ -866,7 +875,7 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>34</v>
       </c>
@@ -874,7 +883,7 @@
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>35</v>
       </c>
@@ -882,7 +891,7 @@
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
Finalizing processing of complete falls
Further developed the processing of the falls
</commit_message>
<xml_diff>
--- a/PIV_Campaign_Processing/Observation_periods.xlsx
+++ b/PIV_Campaign_Processing/Observation_periods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ratzVKI\PIV_Campaign_Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CA47A5-307D-4B29-836A-0150CCD099DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D418B47F-D8B3-4776-9F48-8A3339B9F291}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9530F36F-8309-4E2A-8AEF-06175DE3F285}"/>
   </bookViews>
@@ -516,7 +516,7 @@
   <dimension ref="B1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -630,7 +630,7 @@
         <v>220</v>
       </c>
       <c r="D8" s="1">
-        <v>377</v>
+        <v>396</v>
       </c>
       <c r="E8" s="1">
         <v>462</v>
@@ -644,7 +644,7 @@
         <v>136</v>
       </c>
       <c r="D9" s="1">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E9" s="1">
         <v>488</v>

</xml_diff>